<commit_message>
Get daily reddit data: Tue May 14 08:09:54 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_19.xlsx
+++ b/data/2024_05_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C479"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3032 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1crmr07</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>🌿</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gx9w1qhmc0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1crm96v</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Pasty pale girl neutrals?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crm96v/pasty_pale_girl_neutrals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1crlsbq</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>6 weeks old</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br5y68hw9c0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1crld5u</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>I’m so in love with them</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha8841go4c0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1crlc34</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>I’m so obsessed</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpks07ra4c0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1crkbtn</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They like? </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lblxc8vjsb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1crk2vq</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Floral</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfc4uwlupb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1crjs1r</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Gel nails vs. acrylic gel nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crjs1r/gel_nails_vs_acrylic_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1crjpc3</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons from CVS and a ladybug 🐞 </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m82dbbyrlb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1crjn8w</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>how do these look?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crjn8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1crjly5</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Fue la primera y última vez que me las hice</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crjly5</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1crjbrd</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Went to a new nail place! Got chrome for the first time.</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crjbrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1crj5hw</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Builder Gel Glazed Donut Nails 😍🤍</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksa4mgf0gb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1critu9</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Is it giving Shrek?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opjtpfrrcb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1crit7j</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">broke a nail. can hard gel be applied over it? </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gue9jelcb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1criau2</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Birthday nails! What do we think?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zbum4gj7b0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1cri9x7</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Question on curing with uv lamp</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cri9x7/question_on_curing_with_uv_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1cri5sv</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>my first and second gel-x attempts</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cri5sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1crhrok</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Fill tomorrow!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crhrok</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1crha8m</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Birthday Nails for the month 🥳✨</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5200zc4ya0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1crh617</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Lily &amp; Fox</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crh617</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1crgyqp</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>I made a new manicure for myself, I wonder how you like it</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12afav27va0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1crgy4s</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>My first attempt at 3D water drops on my sisters nails. Credits to meeee♥️</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crgy4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1crg7fb</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>I've never been a French tip girl, but the micro-French/alternative French might be my new fave.</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0795y31foa0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1crfsu2</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>a new set of gel-x nails i just did 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3ky4n2ska0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1crfsj7</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Snail Nail I Made</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crfsj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1crfetf</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>First time getting my nails done in over 6 years. I hate them but are they supposed to look like this??</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fokdxmpcha0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1crfemy</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which order should I use these in? </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6anyat9bha0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1crf2qj</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In desperate need on sheer/nude recommendations preferably non pink. My appointment is tomorrow! My two options so far, OPI 1x Funny bunny and 2x Put it in neutral or DND 867 Pefect Nude. </t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crf2qj/in_desperate_need_on_sheernude_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1crentq</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>P.Shine nail buffer kit</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcelxbhraa0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1creduq</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>in love with these press ons!!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1creduq</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1crdj8h</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>I cut my nails…did I f up?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crdj8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1crctfw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Thoughts girls&amp;Gs🧡</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/is0ija5mv90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1crcp0k</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A simple gel extension + french manicure I did to myself a while back  </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tou9owtnu90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1crcjtf</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Lime Nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crcjtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1crch75</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sncny7zs90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1crcd7a</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>♥️</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eisa4kz4s90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1crc5az</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Newbie here! Is ph bond useful for press on nails?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/durunddhq90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1crb3x8</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Pearlescent nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1k5c8tki90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1craktq</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Do these look too grown out?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1craktq</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1cragmb</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Top coat on press-ons?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cragmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1crab1f</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Is my nail too weak for a new set?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crab1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1cra6iy</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Got them done!!</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cra6iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1cra3fp</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I generally don't care about trends in nails...but I now see why glazed are all the rage! </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrf9jue5b90d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1cr9iz4</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Finally got red again</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr9iz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1cr9db7</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Groovy baby 🪩</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fkqjz0w590d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1cr99en</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Remove Yellowing from Gel Nails</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr99en/remove_yellowing_from_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1cr8r8l</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>They remind me of a red dice 🎲</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr8r8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1cr8nye</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Playing Around with Designs</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpuvj8nw090d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1cr8g54</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X for a wedding this week! </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp3ubnadz80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1cr80dw</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hand painted by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wff765g9w80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1cr7381</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Anyone had succes with non-glue press ons?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr7381/anyone_had_succes_with_nonglue_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1cr6y5l</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Did a whole set with the koi fish and lily pads</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr6y5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1cr6r1l</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Press-On nails all too curved? Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr6r1l/presson_nails_all_too_curved_any_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1cr62e3</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr62e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1cr60xg</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Pink ombré sparkle nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/is68xld2i80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1cr5kx9</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Stained Glass</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp7kfzuwe80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1cr4wnr</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Junji ito nails 🖤</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3awq6cs0a80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1cr4s4u</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr4s4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1cr4n6j</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>I tried gelx for the first time!</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr4n6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1cr4mhd</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Anyone know what this is?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/813ioitz780d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1cr4jh6</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>:(((((((</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f02ey6d8780d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1cr4d1f</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Which nails 1,2 or 3</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr4d1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1cr46qi</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Lumen Nails: Glass Fawn dupe</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr46qi/lumen_nails_glass_fawn_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1cr3mxs</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>How do we feel about clear?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5l20qmws080d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1cr35il</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It turned out great. </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr35il/it_turned_out_great/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1cr2qae</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Base under fake nails? </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr2qae/base_under_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1cr2kqv</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wearing plastic gloves for long periods of time/Need advice </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr2kqv/wearing_plastic_gloves_for_long_periods_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1cr2ctm</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Birthday weekend nails ✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p57chser70d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1cr1v1r</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinions </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3rj2s1pn70d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1cr1jp5</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>sage green chrome gel x</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr1jp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1cr0t65</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>gel lamp suggestions</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr0t65/gel_lamp_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1cr0r6c</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>got my nails done for a music festival</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07ar42ibf70d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1cr0qt3</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Nail help</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr0qt3/nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1cr0jbe</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Pic of my wedding nails!</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m44hnrwmd70d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1cr0idz</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>2nd attempt at semi-permanent</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr0idz</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1cqzdod</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>3D texture</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqzdod</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1cqyqdc</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>5 weeks of growth and I didn't lose a single one. Scary but also satisfying.</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqyqdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1cqykqe</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Christmas Nails 2023</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqykqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1cqyk40</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>New nails 💙</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqyk40</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1cqygfi</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Witchy nails by AJ at Sugar Pop Nails in SLC</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/491vc8rsw60d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1cqxjmh</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Look at my new nails!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k025xnygo60d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1cqxavr</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Should I finished this set?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqxavr</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1cqx5nx</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Sculpted Builder Gel Nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqx5nx</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1cqwoum</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Can I call you 🌹?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqwoum</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1cqwdxv</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>New nails what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpf4blfmc60d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1cqwblb</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Classic nude shellac</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnpmgjnxb60d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1cqvw02</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In my fun nails era </t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qy4mqx32760d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1crmqnq</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat </t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crmqnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1crlyju</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>My first ever real attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crlyju</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1crlk5x</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>I have a 10 month old and I stay up late to do my version of self care</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m4chvh27c0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1crkqmx</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>In honour of the aurora australis 🌌✨</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crkqmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1crkc2v</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>How do we feel about Night Owl Lacquer-in particular cremes and topcoat?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1crkc2v/how_do_we_feel_about_night_owl_lacquerin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1crkfrf</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Night Owl Cremes?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1crkfrf/night_owl_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1crk4p6</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Hello!! What nail polish gives this color??? I've been looking everywhere but can't seem to find one (gel or non gel both okay! preferably one that doesn't require a light haha) :)</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwls9gq5qb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1crjkiu</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Help me choose my last spring manis!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crjkiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1cridsh</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Things I Do during Zoom meetings</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cridsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1crhd5b</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Lipgloss-ish</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crhd5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1crgm0c</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>This color is TOO PRETTY not to post again!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctuobrh2sa0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1crglfp</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>these pictures don’t do it justice</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crglfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1crgd52</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Just A Tint💕</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crgd52</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1crgadb</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Why do big/celeb makeup brands never tackle nail polish?!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1crgadb/why_do_bigceleb_makeup_brands_never_tackle_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1crgac3</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Pure Pandemonium (and Mercury's Tears)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crgac3</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1crg059</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>My first post</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybh7owwlma0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1crfzou</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Mooncat 'Illusionist' velvet style - in love!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/41n37btgma0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1crf6go</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>First Thermal</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crf6go</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1cret17</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cret17/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1crekl1</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Prehnite - Shlee Polish</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crekl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1crdns5</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>I've been slacking...</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crdns5</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1crdhjd</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Never Tide Down, but make it matte ✨️🩵</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3rjd7yu0a0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1crcrxc</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Wasn't super happy with these nails until I saw them glowing. Scroll to see them in regular light</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crcrxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1crcpqz</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Any recommendations for low profile nail charms?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyfwhaktu90d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1crcggi</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>One of my favorite summer colors as a dark polish fiend</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crcggi</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1crce3q</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>♥️</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du04ekrbs90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1crb326</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Nail evolution (backwards order)</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crb326</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1cravwj</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>When you try to get pretty pictures of your manicure, but it looks cooler in car lighting 😬</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cravwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1cras2b</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Zoya Celestia 🤍</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cras2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1cra6g6</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Went with a more funky color combo this time 💚💙💜</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cra6g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1cr8yh9</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Freshly engaged manicure ☺️</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr8yh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1cr8lj3</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Give me grey but make it Spring!</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k814wmff090d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1cr85lf</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>It makes me think of a velour blanket</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr85lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1cr80n9</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Cupcake Polish - what are your favorites?</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cr80n9/cupcake_polish_what_are_your_favorites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1cr7yrr</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">red and pink lightning hand painted by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgr7jbdxv80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1cr7k1x</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Nail polish websites that sell gift cards?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cr7k1x/nail_polish_websites_that_sell_gift_cards/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1cr7gip</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Finally a sunny day so I can show off the glow!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr7gip</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1cr6fvx</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Pool Party 🏊‍♀️🎉</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr6fvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1cr609s</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Naydra</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/opjkn5sxh80d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1cr5yiw</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Why did my top coat (Essie Speed Setter) do this?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dex559clh80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1cr5ngb</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>obsessed 🤩</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04vy0kgff80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1cr5g8y</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Nail polish storage &amp; organization megathread?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cr5g8y/nail_polish_storage_organization_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1cr53eq</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Does anyone collect rare and discontinued polishes anymore? These are in my collection</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr53eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1cr4hxh</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>One coat „Teal no lies“ on my crusty mom hands 🥲</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32zi7pl2780d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1cr449c</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Cirque - Sapphire</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr449c</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1cr3u2i</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Cloud Nine 🌙☁️</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr3u2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1cr3omo</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>New and returning Cirque Vice colors revealed-what do we think?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr3omo</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1cr3e85</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Illimite had some fun polishes</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr3e85</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1cr2b8i</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>New Fav: Lush from Polished for Days</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr2b8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1cr2b1t</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>On today’s episode of “we have that at home”</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr2b1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1cr1rep</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Velour</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr1rep</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1cr1km6</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>The many faces of Airy 💚💛🩷by Polished For Days</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr1km6</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1cr18w5</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>OPI Glazed N’ Amused as a Topper is SO good!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzp1sdh3j70d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1cr175l</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Lumen/Ethereal on HHC?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cr175l/lumenethereal_on_hhc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1cr1218</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need some brand recommendations </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cr1218/need_some_brand_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1cr00p4</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Blue and coral holiday vibes 🌴</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr00p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1cqzvzl</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>My friend asked me if I had any pink to purple shifty polishes.</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqzvzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1cqzp1i</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Is it just me or does Mooncat polish take forever to dry?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cqzp1i/is_it_just_me_or_does_mooncat_polish_take_forever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1cqz1cq</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>🫡🫡🫡</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hqr94cs170d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1cqysjh</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Mother’s Day at the zoo!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfjpmpuqz60d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1cqwkim</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Another fantastic purple - and cheap!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqwkim</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1cqw4pk</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>What do you do when you're disappointed by a new nail polish?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cqw4pk/what_do_you_do_when_youre_disappointed_by_a_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1cqvf4r</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Holographic sticker turned white after applying top coat</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqvf4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1crmg9k</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>2 worlds set and prett in pink</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crmg9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1crls2f</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>This nail design is what first got me interested in nail art</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpln8sbs9c0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1crku7b</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>My recent nail art inspired by avatar the last airbender featuring appa✨</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crku7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1crkqa1</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Cow Abduction</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crkqa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1crkppf</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Frog Skin Nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfm92ukwwb0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1crir6n</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>little details 💕</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crir6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1criptq</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>My most resent design</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1criptq</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1crhz0g</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>All advice welcome! DIY Press-Ons</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crhz0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1crg7al</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Summer vibes 🌴</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crg7al</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1crft7n</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Snail Nail By Me</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crft7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1crdp74</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mate nude </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c44pgefm2a0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1crd5xl</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Hermosas uñitas de hoy!</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p88wd9pby90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1crcmkm</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Neon cherry meets pop art nails</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crcmkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1crbtuo</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Bows on everything 🤍🎀🧸💅🏼</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crbtuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1crbebw</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Citrus and Floral</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crbebw</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1crao67</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Pride Month Nail Art</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1crao67/pride_month_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1crahg0</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Sunday night 💅</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crahg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1cr7zxc</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink and red strikes hand painted by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2rjbx46w80d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1cr701c</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Did a whole set with the koi fish</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr701c</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1cr5rip</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>My very first attempt</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr5rip</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1cr3zrc</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>✨️Sparkly Rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eoicqjwg380d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1cr3wsq</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Nail ARt DESIGN BEAUTY HUB</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wj8u77hf280d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1cr30l7</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Beauty Hub</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fyo7rrgmv70d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1cr15bg</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Butterfly Gems DIY</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cr15bg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1cr0zqu</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A bit messy but I still love them.  </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ws6xan4h70d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1cr0o1l</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>An offering to the garden gods</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cim682nne70d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1cqw7k8</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>First time making 3D designs</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cqw7k8</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May 15 08:08:56 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_19.xlsx
+++ b/data/2024_05_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C479"/>
+  <dimension ref="A1:C643"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8576,6 +8576,2794 @@
         </is>
       </c>
     </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1csf869</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had my first attempt at Gel X nails and nail art today! </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ownvei6oj0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1csf3w6</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Warm and cold 💅</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo2qxsbjmj0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1cseq1f</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Baby blue tips</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cseq1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1csekbn</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Bisexuality Pride</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mi811iyhfj0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1csd10m</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>🐆🍒</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3ouo4tswi0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1csd0y8</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>I’m still in awe</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8qwobzrwi0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1csbpxa</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>How frequently should gel be used ?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csbpxa/how_frequently_should_gel_be_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1csboqx</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>I'd like to do in blue next time. Will it fit?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csboqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1csbcm7</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>I’ve been doing my own acrylics since December, please let me know what I can do better! Always trying to learn</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ya11q8zafi0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1csb7f5</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Birthday nails what yall think</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csb7f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1csb085</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>From a couple months ago! ✨</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8temh4fzbi0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1csaok9</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>any advice on how to shape natural nails?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csaok9/any_advice_on_how_to_shape_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1csad1x</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flt4q0gx5i0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1cs9zkc</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Lil strawberry moment 🍓🩷</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs9zkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1cs9z68</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>One of my favorite polishes 🍀</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs9z68</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1cs9sj2</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>new set 💎</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4473q2is0i0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1cs9k7x</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Any recs for how to get a more natural french mani?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs9k7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1cs9g6e</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>New to DIY nails.</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cs9g6e/new_to_diy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1cs9cmw</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>DND 007 Canadian maple</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs9cmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1cs8jcv</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My second acrylic set ever! </t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs8jcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1cs8efy</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Chrome Set</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48egu3njoh0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1cs8b06</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Graduation Nails for a Friend</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8mcte9pnh0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1cs7yaa</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cs7yaa/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1cs7s0s</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Yaaaaaaaayyyyy 🥰</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs7s0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1cs7iuj</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>My new nails :)</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs7iuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1cs7biq</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>What products would you use to recreate this?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfx1wtv3fh0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1cs77xi</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>My nails are starting to interupt things like typing</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbeqk42aeh0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1cs739q</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>My nail lady is moving and I’m devastated.</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iz39rcx8dh0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1cs6ipy</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ctgoibj8h0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1cs66f7</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Would love tips to help me learn how to do nails for gf</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cs66f7/would_love_tips_to_help_me_learn_how_to_do_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1cs62q0</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Why dont my nails last?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cs62q0/why_dont_my_nails_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1cs61kt</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love simple looks </t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wovku8n4h0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1cs5cau</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink and purple </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39nmslh1zg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1cs5c1z</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">we are slowly progressinng </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/181y8hlzyg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1cs56wq</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>I am in love with my black nails</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lerzkgvuxg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1cs55tb</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I had asked for clear to black ombré, the tech messed it up and showed me and I thought it looked metal AF! I had him do that instead 😛</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs55tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1cs54ea</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Earthy tones?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x5oh9scxg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1cs4x88</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Nail Primer?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cs4x88/nail_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1cs4wdi</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Tattoo manicure 😍</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3j9smvmvg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1cs4vco</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>My bobs my rules 😅</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnxt0n3fvg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1cs46md</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Summertime Sadness</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9nf1kx5qg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1cs45dz</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Loving these colors ✨</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs45dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1cs44lx</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Nail Idea</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlzno5mqpg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1cs42bp</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Love my latest nails. Embracing a bit of design for a change.</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs42bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1cs3yg7</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>May nails 🍉🍉🍉</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksho7anfog0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1cs3r5j</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fancy? </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr8mp9pwmg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1cs1w6p</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>I’m a copy cat…☺️</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lgjv3y69g0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1cs287a</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>What I Got vs. What I Asked For (Inspo Pic: @daily_charme on IG)</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs287a</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1cs2kjw</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>My first time ever getting a design! 🍓</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3laxn52eg0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1cs2eyw</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Manicure advice</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cs2eyw/manicure_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1cs2cu7</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>In honor of Bridgerton S 3</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs2cu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1cs1sea</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>💜❤️</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdfr41tg8g0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1cs1huh</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>May nails 🍉🍉🍉</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksk1dnpc6g0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1cs1cxq</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Ohora Nail Question</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs1cxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1cs1bsh</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New spring nails I did last night. Bf selected the design which thankfully was fairly easy. I love simple dots. </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs1bsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1cr8xp2</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Hema free gel polish brands available to the public?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cr8xp2/hema_free_gel_polish_brands_available_to_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1crb45g</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Help! How can I remove gel nail polish at home?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2f0bipdli90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1crbasw</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Floral Citrus Custom Set</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crbasw</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1crd1oo</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Help please!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ltcfvafx90d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1crgde7</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Hair glue tip from tiktok</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crgde7/hair_glue_tip_from_tiktok/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1cs15cw</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>How common is it to get mold from lifting acrylic?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs15cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1cs0lx7</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>super happy about this hard gel royal blue mani 💙</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79t21ntszf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1cs08oh</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Mermaid lilac</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn496xx2xf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1crh2mx</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>tried coffin nails this time, what do we think?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crh2mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1crh99i</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Nail charm glue</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7nvsh6vxa0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1crij5h</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Is this bad?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crij5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1crnnia</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Am I toast?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxcr7wkayc0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1crpadj</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rejuvenating clear polish? </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crpadj/rejuvenating_clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1crrfcv</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Best long lasting nail polish?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crrfcv/best_long_lasting_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1crvam3</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Black nail polish not transferring</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crvam3/black_nail_polish_not_transferring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1crzu6l</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Nails I did for my birthday💜✨</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fprlr36uf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1crzarr</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>First time applying gel polish myself</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnqycsj9qf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1crz5f6</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> What do you think ?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkvcey37pf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1cryh4t</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Favorite brush on nail glue for silk wrap repairs</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cryh4t/favorite_brush_on_nail_glue_for_silk_wrap_repairs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1crxw7n</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Short-term nails?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crxw7n/shortterm_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1crxs0q</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nothing extraordinary, but did it myself </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w8cdyccff0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1crxnfw</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Super cute nails for my trip to WDW</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trt5kxkfef0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1crxci7</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Cute ant set I did for my friend! Opinions?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lp131o7cf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1crx9fu</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Nails for a show tonight</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86trgwilbf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1crx43o</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>How to stop builder gel nails from chipping?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crx43o</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1crwyc3</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>I’m loving this cute design! ✨</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crwyc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1crwrmn</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Blue magnetic</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crwrmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1crwqnh</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>First Attempt with Soft Gel Tips</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9b0okokv7f0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1crwked</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Baby blues for spring?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ym2rlk9l6f0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1crwifj</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Cat Eye</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2w8bal66f0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1crve63</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Grad Gift to myself! Is almond a good shape for me?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99zdxhyuxe0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1crv03l</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunshine and summer time! </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udsha8iwue0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1crulwl</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Anx13ty made me do it 🥹</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crulwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1crtstf</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>I tried the aura nails!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crtstf</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1crtf7w</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>My first attempt at adding 3D elements!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crtf7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1crt7nj</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>What shape to file</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crt7nj</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1crsqwi</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Did my summer nails</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crsqwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1crslq7</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>First set of gel polish nails. Fluorescent and natural lighting</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crslq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1crs8a8</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Gel Polish Removal HELP!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crs8a8/gel_polish_removal_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1crripc</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Can I use those with gel glue and UV lamp? Sorry Im new to this</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60q9xuxt3e0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1crr9qy</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink always tops the list. </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1crr9qy/pink_always_tops_the_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1crqjiy</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>My first set using a lazy technique</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k5vfmwuud0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1crqdfu</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Save me from wasting money: these aren’t extensions right?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwrexpzatd0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1crpr7u</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>fairy forest nails</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crpr7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1crpfav</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Okay so everyone has been telling me I'm crazy - she didn't refill my biab right?? Got "refilled" a week ago </t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1q1wczjjd0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1cse4ej</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail&amp;cuticle oil </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cse4ej/nailcuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1csey7c</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Hot and cold 💅</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az7n1d1ekj0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1csd02n</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">glowy goodness in motion! </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/usuwac9gwi0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1cscyyl</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>glowy goodness</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cscyyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1csbru1</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Traveling to Japan - Nail Polish?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csbru1/traveling_to_japan_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1csbo82</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Cirque - nsfw jelly</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csbo82</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1csaf4h</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">second desperate plea </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csaf4h/second_desperate_plea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1cs9wl4</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>How to remove peel off base coat without using One kill gel remover from Jello Jello</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cs9wl4/how_to_remove_peel_off_base_coat_without_using/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1cs9s7h</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>serpent venom by cuticula 🐍</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gfwlddp0i0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1cs95g7</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>A mannequin holo for a weekend of wedding guesting</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs95g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1cs8ka2</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Thrift find!</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfas7pjxph0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1cs8gl7</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Rip righty</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbd6tx21ph0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1cs7on3</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Brown liner holo comparisons ?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cs7on3/brown_liner_holo_comparisons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1cs7jd9</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clionadh Cosmetics Forest Flame </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs7jd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1cs7cze</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Formula dupe for cirque shimmers?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cs7cze/formula_dupe_for_cirque_shimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1cs79ak</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Passionfruit vibes 💛</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs79ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1crwz48</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GWP from HHC </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1crwz48/gwp_from_hhc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1cs6umk</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Love an easy pink creme</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs6umk</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1cs58hv</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Advice on mixing colors</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cs58hv/advice_on_mixing_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1cs416k</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Unexpectedly lit combo 🔥</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs416k</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1cs3nov</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Broken Scales </t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs3nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1cs3keh</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Cyborg 🤖</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs3keh</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1cs3j3u</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>I did my nails and I’m getting Cell vibes from DBZ</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs3j3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1cs2rre</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Love this combo 💙</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs2rre</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1cs2n7c</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>What did you buy during the mooncat sale?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cs2n7c/what_did_you_buy_during_the_mooncat_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1cs1xjo</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted my nails white last night and woke up to them turning yellow this morning? They’ve gotten even worse throughout the day.  Why? Looks so bad lmao </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/el8ejhkg9g0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1cs1es5</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Which brand do you think has the most misleading pictures?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cs1es5/which_brand_do_you_think_has_the_most_misleading/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1cs08vp</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favourite Brushes? </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cs08vp/favourite_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1crzv63</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>The Shag</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crzv63</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1crzcph</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Cirque Colors, Time Traveler</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kltsyctnqf0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1crz92p</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Taco Bell summer</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgz7tikxpf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1cryfh1</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Sometimes you’re just in the mood for a polish so neon it makes your eyes hurt!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cryfh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1crxzw8</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Palette for nail art</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1crxzw8/palette_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1crxutx</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Death valley nails- ouzle! </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crxutx</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1crxtqd</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>My gel x base coat won’t come off!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3nxlblpff0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1crxjbf</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>First time trying one of these Magnetic nail polishes</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grakl68mdf0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1crxirf</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Cleaning out my nail polish…</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crxirf</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1crxftu</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Help IDing Color Club Polish</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crxftu</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1crxebc</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>SO EXCITED FOR MY HUGE SCORE!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1crxebc/so_excited_for_my_huge_score/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1crwhmi</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Polish Collection Data</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crwhmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1crwb7c</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>I layered to make these combos and now I need the real thing</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crwb7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1crvqen</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Do I need to buff before base coat?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xx9hj6e0f0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1cru505</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>ILNP deep space</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cru505</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1crtyif</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Queen of Rot - Beesknees lacquer</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crtyif</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1crt2me</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Sad beige office improved with fiery nails</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crt2me</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1crsoju</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>🐟 Catfished 🐟</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3px4gj0bde0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1crr3x9</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Thoughts on the Sassy Saints nail kit? (UK)</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1crr3x9/thoughts_on_the_sassy_saints_nail_kit_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1crr1h1</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Olive olive these colors</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crr1h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1crpznz</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple mani </t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf22od1epd0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1crpwc2</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What a terrible start to the day </t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybv6nggfod0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1crp8dp</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Does anyone know a dupe for Dandelion Clock by Prism Polish?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep6tkwjjhd0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1crclha</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Abstract Nails</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crclha</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1csbxma</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>First attempt at Invader Zim nails</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w19ottp4li0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1csac4d</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Encapsulated Fruit </t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1q26thp5i0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1cs9tly</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>The Nails Bae Gold Chrome Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56udw9r11i0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1cs8i9z</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my second acrylic set ever! </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs8i9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1cs8bku</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Is it safe to glue on plastic nail charms on natural nails?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1cs8bku/is_it_safe_to_glue_on_plastic_nail_charms_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1cs64fq</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m in love 😍 </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loqjucma5h0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1cs4zn1</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Curing after chrome powder</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1cs4zn1/curing_after_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1cs3sni</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Lime Nails</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs3sni</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1crwooo</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bruji nails!!! </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mp9va8h7f0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1crtg43</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>My first attempt at some 3D elements!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1crtg43</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1crswiw</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Glacier? Blue lagoon?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efiuvgexee0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1crohkg</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Its a Fairly Odd Set 😏✨</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pojorgbs8d0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May 16 08:07:31 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_19.xlsx
+++ b/data/2024_05_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C643"/>
+  <dimension ref="A1:C826"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11364,6 +11364,3117 @@
         </is>
       </c>
     </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ct73wb</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any decent nail techs in Ely, Cambridgeshire </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct73wb/any_decent_nail_techs_in_ely_cambridgeshire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ct6xaw</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Matching nails with my partner in crime 😎🥰😬</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmj4t7a7lq0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ct6vtn</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>What is the difference of russian manicure and a normal?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct6vtn/what_is_the_difference_of_russian_manicure_and_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1ct4uyr</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Advice Greatly Appreciated!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fpld7newp0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1ct53o7</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Inspired by pokemon</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv72b5l2zp0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1ct5epw</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are gems on nails worth it? </t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct5epw/are_gems_on_nails_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1ct5y43</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Engagement Nails</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct5y43/engagement_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1ct6imv</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>How to avoid tops of gems falling off?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5thk6pvfq0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1ct6ns3</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>How to donate nail press ons??</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct6ns3/how_to_donate_nail_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1ct6k3c</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did my own builder gel nails + nail art! </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct6k3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1ct5yya</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Been practicing my press on technique and I can see definite improvement!</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct5yya</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1ct5mae</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Gel or dip</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suq6v8iy4q0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ct53ai</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Went full Disco</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zyh5ocyyp0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ct4q2h</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Cute Easter set! (Better late than never)</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct4q2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1ct4o97</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Who loves Etsy glue ons?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scmfwl0dup0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ct4nce</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Changed my nail shape</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct4nce</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ct4jgt</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink flowers </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w61nygiwsp0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1ct4diu</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Appreciation for my acrylics please! I love the colors!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ddt0n74rp0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ct42ll</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Question about gel x nails</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct42ll/question_about_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1csz8us</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Will a Nail Tech Install Fake Nails on Bare Nailbeds?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csz8us/will_a_nail_tech_install_fake_nails_on_bare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ct24xx</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Advice for starting nail IG, TT, etc</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct24xx/advice_for_starting_nail_ig_tt_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1cseklv</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I got the past few months :) I love my manicurist! </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cseklv</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1cshg51</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Preparing for success as a nail tech in the US, coming from Vietnam</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cshg51/preparing_for_success_as_a_nail_tech_in_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1csnkt4</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Where do you get you press ons when most nails from Etsy are Shein/Temu resellers :(</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csnkt4/where_do_you_get_you_press_ons_when_most_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1csqg7n</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>How do I stop my nails from yellowing when I wear clear/irridescent polish?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csqg7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1csri8f</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Nail Opinions</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywebu6a7sm0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1cssh77</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>New nails who dis💅🏼</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cssh77</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1csu51l</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>How long do your full coverage tips stay on with the glue you use/how often do you change sets?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csu51l/how_long_do_your_full_coverage_tips_stay_on_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1csuihz</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Cutest nails I’ve ever had!!Inspo from nails_by_miaaa on TikTok ❤️</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csuihz</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1csuu5k</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Allergy options?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csuu5k/allergy_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1csvy2h</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>How do you get rid of that tough skin on the sides without cutting off half of your finger?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onfdghuwon0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1cszpm2</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Twenty One Pilots Clancy inspired Nails</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cszpm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ct34rj</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Getting outta my comfort zone</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct34rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ct2gko</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What kind of nails should I get for my job? I work both truck and Cashier. </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct2gko/what_kind_of_nails_should_i_get_for_my_job_i_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ct30ti</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>My recents 🩵💖</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct30ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ct2fyt</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilnp wildflower collection </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjipzx818p0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ct2a1v</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>My acrylic snapped off, what should I do!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5ywzt1i6p0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ct24zw</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love a milky white </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrkyj0t75p0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ct1w8k</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Is it safe to use a UV Lamp with a magnetic nail display?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct1w8k/is_it_safe_to_use_a_uv_lamp_with_a_magnetic_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ct0yr3</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>I miss my long nails 🩵</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8jnbwekuo0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1ct0sfp</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Show me your best or craziest nail set .Here’s mine 😝😍</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct0sfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ct0kwg</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Honest Opinion</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t63twn72ro0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1ct0i91</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>🔥🔥</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2byaqardqo0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1ct0dbd</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ct0dbd/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ct0cv7</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Summer 🌞 Pink &amp; Purple 💜🩷</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct0cv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1ct0c0x</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>💜💜💜</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scp4dg9soo0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1ct09ze</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7qtdsl7oo0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1cszhpx</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Don’t rain on my (neutral) parade! 🌧️ 😉</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vdl6g49ho0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1csyse0</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">trying to find flowers that match your polish </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csyse0</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1csynmu</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Yes, they glow in the dark!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csynmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1csyjy6</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>the nails vs the mess</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csyjy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1csydzq</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>3rd time doing them</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csydzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1csycvm</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>🦋🦋🦋🦋</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csycvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1csxihi</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Recommendations for chic / classy colors?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csxihi/recommendations_for_chic_classy_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1csxh8v</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Colorful snake prints for Megan Thee Stallion last night 🐍</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csxh8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1csxfwl</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Best kind of gel for healthy nails?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csxfwl/best_kind_of_gel_for_healthy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1cswo9y</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>How to take off gel extensions while keeping the fake nail intact?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcapychiun0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1cswn90</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>been loving press ons lately !</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hp4od5aun0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1cswcef</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Had a little fun with my new matte top coat</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ghtqzqzrn0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1cswb0w</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>🐆🍒</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzrn5ajprn0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1csw9eh</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>I decided to treat myself - what do you think (first time posting here🤭)</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6tc5p1drn0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1csw567</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Can gel x be reshaped at fill?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csw567/can_gel_x_be_reshaped_at_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1csw1e0</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>what do you do while the nail tech is working on your nails?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csw1e0/what_do_you_do_while_the_nail_tech_is_working_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1csw0hw</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to grow nail beds? </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csw0hw/how_to_grow_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1csv99d</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Wasn't super happy with my "fun" birthday nails till I saw them glow. Scroll for the glow</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csv99d</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1csv732</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I think liberties were taken in the photos on Amazon.</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjqneni0jn0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1csurgs</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>help with water decal!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0qv98ohofn0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1csubka</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>If you want only a clear coat, do you do only top coat or only base? Or both?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csubka/if_you_want_only_a_clear_coat_do_you_do_only_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1csu3eu</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>I’m just OBSESSED with how this looks</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csu3eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1cstuek</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Flower Child 🩵 Absolutely stunning! That glow is next level! ✨ Bonus pic of Willow on my toes! Perfect spring green and I think it will work well for Halloween too!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cstuek</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1cstt30</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unintentionally matching my shoes, but I'm here for it </t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cstt30</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1cstsw4</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Juicy Fruit Salad Nails - Summer ready ✅️</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cstsw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1cstqsh</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>How much more are you willing to pay for a scheduled service provider to come to your house for a mani? Pedi? Or both?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cstqsh/how_much_more_are_you_willing_to_pay_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1cstd3q</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Aren't they divine?! 💅</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aye00kye5n0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1cstc2o</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Nail Day</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cstc2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1cssfwz</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Blueberry milk 🫐🥛</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4yrqvqkym0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1cssenr</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Red stiletto nails done myself (and matching toes)🩸🖤</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh214zjbym0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1css5xj</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>I finally did my dream set</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1css5xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1css3ci</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Thoughts on Shein nail products?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1css3ci/thoughts_on_shein_nail_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1csrxzc</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Blue, coral, and pink Skittles nails</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxc53374vm0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1csrgh2</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Where to find nail expo?? That has Korean and Japanese gels</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csrgh2/where_to_find_nail_expo_that_has_korean_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1csr56m</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Fresh and simple 🤍</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aml8spxjpm0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1csndbs</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Aya Takano inspired set ❤️</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kp64r4lxl0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1csr01t</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Bsf asked me to make her bridal nails and I feel so special 🥹 (+ bridesmaids)</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csr01t</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1cskwbi</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Recently got bling for the first time and am looking for inspo. Can I see your favorite bling ideas?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln2jtdvkel0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1csqu67</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Went with a matte look today</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyl1qppanm0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1csqrto</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loved this new Gel polish </t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csqrto</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1csqgs7</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Best Drill and Gel Set</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csqgs7/best_drill_and_gel_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1csq87y</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>I would like to thank my nail tech, cuticle oil, and The Gel Bottle for this length retention✨</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csq87y</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1csq3v2</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Why do nail techs hate doing really short fake nails?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1csq3v2/why_do_nail_techs_hate_doing_really_short_fake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1cspzfr</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Nail growth tips and products recommendations?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpb4diy0hm0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1cspzfd</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>I asked my manicure for a nice and tender design :)</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcdr1er1hm0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1cspz76</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What vitamins/supplements should i start taking for healthier nails? </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cspz76/what_vitaminssupplements_should_i_start_taking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1csoy5q</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>First set of nails ever</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwf72k6d9m0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1csov6h</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>some springtime frenchies :) feat. pup</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csov6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1csoufj</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>First time doing gel x and 3d art myself</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn9t1qfm8m0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1csool2</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>What do we think of this color?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5srldnd7m0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1csoksk</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Wanted a little extra “umph” with my nails this time (cuticles are terrible, I’m a picker lmao)</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1feu7zul6m0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1csnykc</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtg4i9jz1m0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1csnfh0</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Green cat eye nails. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s0r7ff11yl0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1ct70iy</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Nail bruising?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct70iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1ct5q66</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Can someone help me solve this bizarre mystery? Why did only my fingernails turn yellow? Info in comments.</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/hHnxX12.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1ct5grl</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Broken nail pls help!!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct5grl</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1ct5ebn</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Tropical vibe has me ready for a vacation!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct5ebn</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1ct56s9</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s your go to power color? </t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ct56s9/whats_your_go_to_power_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1ct3k5n</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Swatches all my polishes and I think I officially need to put myself on a no buy for the cool colors 😂</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct3k5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1ct38zu</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Curious about what polishes people buy...</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ct38zu/curious_about_what_polishes_people_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1ct2r01</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Inspired by my garden today</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct2r01</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1ct2jq0</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>✨50 Shimmering Years✨</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct2jq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1ct2bs1</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>This polish is really hard to photograph</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct2bs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1ct26dn</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Advice for starting nail ig/tt/other?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ct26dn/advice_for_starting_nail_igttother/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1ct1tnu</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Seeking sheer brown nudes</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ct1tnu/seeking_sheer_brown_nudes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1ct1lye</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Did prom nails! Not bad for my first set in months 😂</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct1lye</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1ct1ctz</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cheap or expensive polishes when starting as a beginner? </t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ct1ctz/cheap_or_expensive_polishes_when_starting_as_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1ct1bzy</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I posted my new mani in another nail sub because I'm on the fence about them &amp; I got told that the application was AWFUL. 'Did you pay for those? Because if so...yikes'. y'all I did them myself 🥲🥲🥲 are they really that bad?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mr790uzxo0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1csm8qa</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Picnic Time!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csm8qa</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1ct0f1t</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Summer 🌞 Pink &amp; Purple 💜🩷</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct0f1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1ct0ac8</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>I really enjoy this combination with a couple solar polishes</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmzkjepboo0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1cszo3q</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone posted here recently asking why Kelli hasn't been reviewing Cirque Colors ... </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0d0033tio0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1csz522</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Ethereal does not miss</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mm5fo9s7eo0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1csz24l</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Sally Hansen x Ring Pop</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t6cohuido0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1csyx07</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Letting My Nail Artist Decide 🩷🤗</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csyx07</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1csyvsk</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the square glitters remind me of the PS2 start up screen </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csyvsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1csymm7</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Swatch comparison request!</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csymm7/swatch_comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1csykv6</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brands that have good thermals? </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csykv6/brands_that_have_good_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1csyfiw</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mileena wins ✨💜 </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csyfiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1csy4o6</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Definitely not taking nail pics at work</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csy4o6</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1csy3do</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Which Essie top coat is your favorite</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csy3do/which_essie_top_coat_is_your_favorite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1csxppu</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>I finally understand why people like jellies</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e39cutvg2o0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1csx6hj</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>bluebell is so worth the hype</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csx6hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1csx43i</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat - Stumped. Anyone else get one that looks like this? </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csx43i</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1cswz8f</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>I was ✨influenced✨ (first-time poster)</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti7q5ho5wn0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1csvnod</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Our Laughter Carries on a Warm Wind</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csvnod</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1csuqr2</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the wildflower collection from ilnp ❤️ </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcm5suslfn0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1csugfr</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Sunkissed on a cloudy day</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csugfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1csu5bu</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Tequila sunrise ☀️</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csu5bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1csu38h</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>How the heck to do funny bunny/bubble bath</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csu38h/how_the_heck_to_do_funny_bunnybubble_bath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1cstrz6</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>This addiction is expensive early on</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cstrz6/this_addiction_is_expensive_early_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1cstru4</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Flower Child 🩵 Absolutely stunning! That glow is next level! ✨ Bonus pic of ILNP Willow on my toes! The perfect spring green and I think it will work well for Halloween too!</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cstru4</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1cstjxx</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>I don't even know what happened 😭</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftfl9oxq6n0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1cssqd9</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Enid</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cssqd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1cssf2r</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Question about cuticle oil</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cssf2r/question_about_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1csrwf1</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>🌈Lemon sibling skittle!!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csrwf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1csrrg0</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>'Outta The Morbs' Blue</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csrrg0/outta_the_morbs_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1csqckx</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>My dog photo bombed my nail pic 😂</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez1zezipjm0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1cspoh0</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>In love with this reflective beauty 😍🥰</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cspoh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1cspksn</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What brand do you think has the most ACCURATE photos? </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cspksn/what_brand_do_you_think_has_the_most_accurate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1cspgdw</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Too hot for thermals 🫠</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cspgdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1csoo3p</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Looking for an office appropriate thermal?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csoo3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1cso9kv</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Molten Lava lives up to the name!</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwh9kgy84m0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1csnqhh</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Don’t do your nails at 12am in bad lighting!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csnqhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1csnn2d</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Neons! (Pink 🩷)</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csnn2d/neons_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1csnahl</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Neon yellows with the best formulas?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csnahl/neon_yellows_with_the_best_formulas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1csmsm9</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>BKL - Cheers to 5 Years</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csmsm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1csmiup</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Stagnant Water</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vk6unxj9rl0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1csm15p</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>The many faces of Treachery in Blue</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csm15p</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1csm13d</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Some finger swatches of sparkly and glowy polishes</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csm13d</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1cslwmb</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>I layered a glowy polish over a thermal and I love it</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cslwmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1cskwl9</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Stranger Tides </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cskwl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1cskib3</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Sometimes a basic red is just what you need</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cskib3</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1csj7ui</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Just wanted to show you guys the disco ball vibes! ✨</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/em090s3ozk0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1cshz5a</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's time for neon greens again! </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cshz5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1csh7vb</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Painted these cute watermelon nails for summer-y vibes</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csh7vb</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1csgooz</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>HHC order to Europe Question</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1csgooz/hhc_order_to_europe_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1cs0m2v</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>First ever attempt at nail art 🙈</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cs0m2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1ct7f2h</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Shadow the Hedgehog (hand painted) 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zrt5bc4orq0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1ct5ubn</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Does anybody know of any silicone molds that have dragon scales like these? Not sure where these pics are from as my girl sent them to me</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct5ubn</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1ct5djg</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Cat eye gel for this week</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct5djg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1ct5d40</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>My set for this week ✨</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hsr23aez1q0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1ct39xl</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Swipe for flash ⚡️</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct39xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1csxjqo</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Gorgeous and Dangling Truck Nutz for Women</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csxjqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1csvgse</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First or second for the next manicure? Also, I'm wondering which shape is better for my hands. Thanks in advance! </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csvgse</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1csumbe</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>My fun short set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hy3x4yhoen0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1csu69z</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic flowers </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0omhg2nfbn0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1cstta7</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>First gel set for a friend!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izlf8ofs8n0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1cssqet</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Ocean blues!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cssqet</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1csqt9v</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried more nail designs with pigments! </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc8wy8m4nm0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1csoh1o</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Mulan nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csoh1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1csn9lg</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Eras Tour Vibes</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csn9lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1csllpg</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Froggy I Made</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1csllpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1csk5wk</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Gel Polish</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1csk5wk/gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1csihqg</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Wish you all gold</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1hbjj7llsk0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1cshzda</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Feel so summery ! 🌷</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cshzda</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May 17 08:09:01 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_19.xlsx
+++ b/data/2024_05_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C826"/>
+  <dimension ref="A1:C973"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14475,6 +14475,2505 @@
         </is>
       </c>
     </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1ctzrgs</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Nails😆</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5tkhppd0y0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1ctz6x1</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>My ex-coworker did my nails!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctz6x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1ctyyz4</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Nails for Teacher Appreciation Week!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctyyz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1ctxeqq</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my32n7ic7x0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ctx8rk</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Acrylic nails popped off :/</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ctx8rk/acrylic_nails_popped_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1ctvx0h</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Longest I’ve grown my nails, from a former nailbiter</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0vapt87rw0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ctvwte</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Too pink?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yn2yvj4rw0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1ctvov4</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails are pretty ? 😍 </t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qa1x4r6yow0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1ctvmpc</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Cherries and 90’s “Jazz Cup” themed nails.</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctvmpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1ctvhsw</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>In love with my new Manicure!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qnodqjrmw0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1ctv47i</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>A lil SpongeBob moment 🪼</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfapz82hjw0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1cttxjt</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can't stop staring at them </t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qdu6dy28w0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1cttuq8</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Cheers to a new set 💅✨</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyb5ciid7w0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1cttgo8</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Did gel nails after so long not doing them</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyf51v9q3w0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1ctt2mv</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>This sub the past few weeks 💅</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctt2mv</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1ctt24t</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first gelx try </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfkd0tnxzv0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1ctsn2i</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Realistic press ons? </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ctsn2i/realistic_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1cts86w</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new press ons girlies </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zqjhgf7sv0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1cts5ki</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>got my first nail extensions ever!</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgjm3zejrv0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1ctrnak</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>My fav nails i’ve gotten</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctrnak</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1ctr6v1</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>First time doing gel extentions and nail art, dripping rainbow tips. Be gentle with me, I tried my best! &lt;3</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctr6v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1ctr5zb</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Really bummed with how these turned out, can I fix them? Gel X done by me.</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctr5zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1ctr4p9</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Seashell pressons</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctr4p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1ctq80b</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>first time doing press ons, anything i can do to improve?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctq80b</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ctpxr6</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>🐜🐜🐜</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp0l69rd8v0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1ctpt21</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made a set of three pastel sets </t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emjl5bab7v0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1ctmgdm</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Small nails help!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ctmgdm/small_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1ctmqc5</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Nail issue</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53eiqp49ku0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1ctn947</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>got bridgerton inspired nails for season 3 release! 🌷🎀</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctn947</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1cto1pk</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>7 weeks of growth 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgdirgsftu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1ctozj5</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Hard gel overlay?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ctozj5/hard_gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ctoxy9</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Gel or acrylic? and why?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctoxy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1ctowox</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>I have very wide nails, so I've always been reluctant on getting my nails done, hoping someone with similar hands can show me what they look like when you've gotten them done</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5liwv7440v0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1ctow2d</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Can I do gel extensions if my nails are detaching?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctow2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1ctoqti</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>First time I’ve had my nails done in 10 years!</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctoqti</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ctoja1</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today was doing a design with my non dominant hand day </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qib83xf2xu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1ctocp3</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Neon pink french drip</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnhsgpvpvu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1ctnrlz</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>ITS A MATTER TOP COAT. TWO LAYERS. THEYVE BEEN UNDER THE LIGHT FOR LIKE THREE MINUTES TOTAL. WHYY ARE THEY STILL SHINY. side note my nails are very durable</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x8jl8ysgru0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1ctng6g</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set today </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6zdw7q7pu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1ctmxpp</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Trying my own sets, whatcha think?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ph1mpcvnlu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1ctmllk</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Got these last year happen for an Anubis custome, current made me think of these!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyrwws6dju0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ctmg11</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>👻</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctmg11</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ctlr02</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>A SpongeBob themed sunset</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctlr02</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ctlj1q</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Cat Eye Gel</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctlj1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ctkpmd</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>In one coral color</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/anx7hz836u0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1ctk3p7</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Should I go back to the salon and get my nails shortened?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9udm01tn1u0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ctjycp</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Needing builder gel tips or recommendations </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftloeunl0u0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1ctj8u9</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>my nail tech after saying she's "terrible at nail art":</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/808gstpgvt0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ctitfm</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>🧡</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/666aoe3ast0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1cti6rq</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>New Nails this Week!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijn9v6fmnt0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1cthr0w</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Best Gel Polish Strips</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cthr0w/best_gel_polish_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1cthoug</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>In a pinch for time so I did some press ons. Had to add a little extra.  imPRESS press ons🌟</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dffmz7i1kt0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1cthnpp</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing gel nails myself </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4e35pxsjt0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1cthfpo</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>My daughter did my nails. What do y’all think?</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae5r9li5it0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1cthe2p</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can we please take a moment to appreciate how absolutely talented my nail tech is </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbxvvcttht0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ctgwxe</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Low quality pic but u don’t have to zoom in to see em they are that pretty 😭 not my work obv</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctgwxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1ctgv5w</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>me n my besties nailz!!!</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctgv5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ctgrle</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>First attempt at rose quartz style nails, but my sheer and jelly polish is coming out quite opaque still. Any pointers?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s1zm0i52dt0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1ctgqlq</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Shade match please</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t72bz7btct0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1ctfw5n</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new set loving it 😍 </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckur0mjd6t0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ctfn4e</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>It’s a lemon party. 🍋</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctfn4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1cteymz</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>🩵🩵</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cteymz</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ctdtk3</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some fun bright blingy summery nails </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2v30mao5qs0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ctdjrx</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Pretty sure there’s a ring 💍 in my near future so I’ve been dusting off my nail skills.</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctdjrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ctdd40</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>I love them that delicate ❤️</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8flobb4pms0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ctc9ok</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Amazon stickers for the win</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ol8vic9ds0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ctbrr4</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Freestyle</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odmrfwvj8s0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ctbp2u</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>My super short almond nails that I am loving!!</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzlwzbpv7s0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ctaxhm</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>It's a lovely color and length, and it matches the color of the flowers. What do you think?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgq0sgmwzr0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ctai3v</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Summer nails - give me inspo!</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ctai3v/summer_nails_give_me_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ctabr0</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>bouncing off another post</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfmyv1omtr0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ct9otf</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>My newest set inspired by creatures of the Cambrian Explosian and the cover art for "Oral" by Bjork ft Rosalia. By okenails in NYC &lt;3</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqcd7qx3mr0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ct8bm6</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Black and Red</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct8bm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ct824f</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I painted Larry from Sally Face </t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct824f</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ctzsxz</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Help, I am head over heels</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctzsxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ctzqt3</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Had fake nails for my wedding...couldn’t get them off till 2 weeks later and now my nails are possibly moldy….how freaked out should I be? 😣</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctzqt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ctydr9</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>natural nail / newbie help</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctydr9/natural_nail_newbie_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ctycdg</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Mooncat - Cosmic Cowboy</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctycdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ctxphx</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Colores de Carol sales?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctxphx/colores_de_carol_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ctxbs8</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Nail swatch dot recommendations</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctxbs8/nail_swatch_dot_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ctx0ns</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Spring is almost over, but these are my February manis 🤪</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctx0ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ctw0gc</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>oh whoa whoa, that Lurid glow tho ✨🎆💡🩷💫</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4wkhmc7sw0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ctvxuo</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>I ended up deciding I needed to redo my mani for my own peace of mind, lol. I'm every bit as in love w/ this color &amp; this time I'm happy w/ the job I did as well. Proud of myself! Also included some Day 1 pics from my biting recovery, since so many of you were so kind :)</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctvxuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ctvava</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid Bait </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctvava</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ctv9j8</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Finally catalogued my collection! You’ll never guess what my favorite color and brand are 😅💙</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfvx9bwukw0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ctuxko</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Yes I took these photos at work, what about it?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctuxko</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ctuiq9</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Best line I've ever achieved</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctuiq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ctudd2</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Every time I've tried to recreate Jinx's nails in Arcane, my weak and flimsy nails have broken. This is my attempt to break the curse. </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe3obe97cw0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1cttzwy</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>I think I found my favorite combination (and it glows in the dark!)</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cttzwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1cttyd2</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Dragon Scales 🐲🐉</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7og3hd6b8w0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ctsbco</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>ABCs of polish! P is for Pahlish.</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1ixuxy1tv0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1cts1de</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Help! What could be causing this damage 😭</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onacpm7hqv0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ctrn1s</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Feeling a little Froggy</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctrn1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ctrluo</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Partly Sunny from Olive Ave Polish</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctrluo</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ctr92k</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse plus a layer of ILNP Ruby for an accent nail 💋</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctr92k</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ctr2eb</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Just got my DVN Order</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfh9rzovhv0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ctqzg6</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>₊‧*ੈ✨ Aurora Beam ✨*ੈ‧₊</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctqzg6/aurora_beam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ctonr9</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Ethereal - Chihiro</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ktzfucx1yu0d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ctof5x</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>There's just something about the stove hood lighting</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctof5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1cto85w</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Dupe for Lights Lacquer’s Catch Me in Capri Collection</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cto85w</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1cto2xe</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>There was an attempt</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3xaru2ptu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ctnuai</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Glimmer by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eiay0ssxru0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ctnjzs</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>bridgerton-inspired nails for s3 release! 🌷🎀</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctnjzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ctniqr</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Me: I’m going to only buy unique colors to keep me collection small, Also me:</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqmojboqpu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ctng94</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Such a beautiful blue!</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vl6iy59pu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ctnan1</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>If your labels do this it was your nail oil!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tg5rd6t4ou0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ctn3l3</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Are one of my Nails Inc glow polishes defective?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/potW4LI</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ctk7ju</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Trying some simple nail art :3</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1s302vg2u0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ct32na</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>First Mooncat Haul!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct32na</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ctmh9u</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>ILNP -Sea Glass</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ys9fl6yjiu0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ctm2s0</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Favorite apps</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctm2s0/favorite_apps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ctly2m</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Today someone said it looks like I got my nails professionally done and that was nice</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctly2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ctlv0r</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Tried painting some jelly flowers</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctlv0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ctl91y</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>This polish is worth the hype.</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctl91y</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ctl38n</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Our laughter carries on a warm wind</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctl38n</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ctjy5t</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had a bad break so decided to chop em all! I love me some shorties! </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j819ex7k0u0d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ctjnxx</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>OPI Malaga Wine</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctjnxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ctjfr8</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Solar vs Thermal</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctjfr8/solar_vs_thermal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ctjbfy</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know of a clear black speckled eggshell  nail polish? </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctjbfy/does_anyone_know_of_a_clear_black_speckled/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ctj5e3</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Just when you thought "prestige" brands couldn't get any crazier  ($57 for disposable nail files)</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hotw0osut0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ct6toy</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>The Good Color Combination</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ct6toy/the_good_color_combination/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1cthrew</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for Mooncat Alien Invasion? </t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cthrew/dupe_for_mooncat_alien_invasion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1cthdnf</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>ILNP shooting star, so pretty!!!</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xqmjgpqht0d1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ctgcup</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>I'm blue, da ba dee da ba diiii</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4agaxn1at0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ctfccr</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Londontown polishes</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctfccr/londontown_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1ctdvz1</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Sundown Socialite 🌅</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctdvz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ctdi2o</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Question about carrying nail polish in checked baggage</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctdi2o/question_about_carrying_nail_polish_in_checked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ctdgrx</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Looking for nail polish that looks like concrete!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ctdgrx/looking_for_nail_polish_that_looks_like_concrete/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ctcyzb</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>When you can’t find the perfect shade and you end up mixing your own Franken-polish</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9k8wkkiejs0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ctco4p</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Mermaid Bait is EVERYTHING</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctco4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ctc8pz</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Well my Mooncat order arrived </t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8np2d22ds0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ctbuna</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Loving the effect of this topper!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctbuna</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ctup3q</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Presson nails </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61fuqjjdfw0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ctt4it</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Played around with some designs 😁</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctt4it</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ctp5p9</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>The Nails Bae Gold Chrome Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2crmxja52v0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ctnerf</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>bridgerton inspired set for s3 release! 🌷✨</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctnerf</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ctmeei</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m not a nail artist but it’s fun to try some new things </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctmeei</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ctlsb0</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>A SpongeBob themed sunset</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctlsb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ctki2l</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>I STILL CANT GET THESE TECHNIQUES FOR THE LIFE OF ME</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxe69qcm4u0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ctjrxr</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Demon Slayer Challenge</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87uicrs8zt0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ctiocv</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Been years since I took time to do my nails. Did I do ok?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zv2h3pd9rt0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1cthijc</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>ready for insanity?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9srwlm2qit0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ctgdan</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Which set should I wear first? 🤔🤩</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ctgdan</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ctf663</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Do these press ons look fake?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oedemwos0t0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ctemc0</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>LV</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65btdk1jws0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ct81r9</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted Larry from Sally Face </t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ct81r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ct7v4i</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Here, the ones of us who love fuchsia</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17szaxqnxq0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May 18 08:07:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_19.xlsx
+++ b/data/2024_05_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C973"/>
+  <dimension ref="A1:C1135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16974,6 +16974,2760 @@
         </is>
       </c>
     </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1cusbwu</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Tonight's press-ons</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cusbwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1curshl</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice please! </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d0pwf0tz41d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1cuqqzq</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Maelstrom from Mooncat is mesmerizing! 🥹</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuqqzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1cuqovk</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Love gray &amp; shine 😍</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeyaza9dm41d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1cuqi1d</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>nail prepping when you have sensory issues?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cuqi1d/nail_prepping_when_you_have_sensory_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1cuq471</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Tortoiseshell</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/849sdmbjf41d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1cup98q</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>For Mental Health Awareness Month.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqrkq3e0641d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1cup7pq</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling uninspired, any suggestions? </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6cfhxkj541d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1cuoxt4</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set done by me </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuoxt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1cuomb1</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2nd try at gel and acrylics </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl3x6aaaz31d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1cuol9z</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>My nail broke.</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuol9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1cuojm2</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Mediterranean vibes</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuojm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1cuoipj</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Strawberry design from a while back 🍓🌼</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e21q2e29y31d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1cuo57h</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time in awhile and im really excited on how they turned out 😊</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuo57h</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1cunsud</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Love the sparkle</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ieao44g2r31d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1cundz5</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>New set turned out great!</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2aylgwym31d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1cuncqj</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>How’s this shape on me?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h5lazfnm31d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1cumh7m</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>O.P.I.</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zp516w79e31d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1cumh0e</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Spring mani</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m6pcee7e31d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1cumgjk</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I’m in love! My nail tech kills it every time ❤️🎱🍒</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w94wnba3e31d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1culwsg</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Another beautiful color by DND 🩷</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lod1d5xw831d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1culwp0</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Currently loving these colors!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1culwp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1cult3n</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62xzfi70831d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1culgr3</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Is this odd? First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1culgr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1culcia</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>🖤&amp;🤍 wrap-ons</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmwbd7xm331d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1cukjhb</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Bought this nail kit and for some reason I feel like none of the nails fit my middle or index finger</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivvwc6h9w21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1cukjgo</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>I came to show my mom's progress compared to last time! she is a genius</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5c1b5w3w21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1cuk17n</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>strawberry nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwc92xwtr21d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1cujy3q</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Lil vampy 'lettos</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cujy3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1cujqjm</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>By these little bubbles?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/des085xap21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1cujou5</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Summer Gel</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cujou5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1cujmed</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Bf’s money well spent</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cujmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1cujc2d</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>‘Lime Cordial’</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z65060lwl21d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1cuj3od</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>36M, friend gave me my first ever manicure, asked if I wanted polish as well and I said "Sure, why not?"</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88yzp32vj21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1cuivag</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>strawberry girl 🍓</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7lyv2qxh21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1cuirdr</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>birthday gift for a nail tech?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cuirdr/birthday_gift_for_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1cuicjo</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Do you like my nails? I did them myself</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30qnjrepd21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1cui35w</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>princess pink</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugrn2qwib21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1cuhzwt</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>pink in different intensities! love!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emy5ddqsa21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1cuhynt</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>I can’t decide but I’m leaning toward the third. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuhynt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1cuhurz</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails and my skinfant </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biyjlqvn921d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1cuhp1v</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Anyone know why my Polish is going so streaky on my natural nails? (Extra: is this polish a good colour on my nails?)</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mehwname821d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1cuhhcs</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>so how come I just now figured out I could apply pre painted french tip nails GEL X style? :D</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0lbjbnq621d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1cuhdqs</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Mardi Gras Nails</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qdu9i3x521d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1cuhbq3</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>I see all your gorgeous and clean manicures looking all professional, and raise you my 'oh shit I need to paint my nails before I leave tonight' ripples and waves.</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mi8tk6h521d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1cugwnx</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>White stuff around my press on nails</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cugwnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1cugp3w</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Blue simple</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qbqqk8j021d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1cugouu</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Peel off liquid mask</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whevz7qh021d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1cuglbm</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>What to ask at the mail salon for ‘glazed’ nails?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/py8853vpz11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1cughlu</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>i love my new tech</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cughlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1cufy8x</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Nude cat eye</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cufy8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1cufv4p</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Does it look like chrome to you?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3dyrqo0u11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1cufqvw</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>This effect is the most!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1j5ej53t11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1cufggd</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Worst nails I ever got + rings of fire</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cufggd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1cuf6g6</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own gel nails in a vampire (black-red gradient) look. Picture with and without blitz </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnwkxjlso11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1cuehg7</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Why are Kiss press ons RUINING my nails?!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23ag47joj11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1cue5wo</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Harry Potter nails</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cue5wo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1cue3de</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Which shape is looks best on me?</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cue3de</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1cue1se</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>i love this glitter</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phiq5qujg11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1cudyff</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Pink BIAB 💖</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjd460qtf11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1cudxa5</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Manicure</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbz2639lf11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1cudty6</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Press On Nails - help!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cudty6/press_on_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1cudp7w</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>metal ore</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cudp7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1cud9dr</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Tips for getting gel polish off my cuticles?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cud9dr/tips_for_getting_gel_polish_off_my_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1cucsp0</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Kiss Impress in "Visions", #91375</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vf1cgnd8711d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1cucp8y</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Adhesive or nail glue for press ons?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cucp8y/adhesive_or_nail_glue_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1cucmdn</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Tried short nails and my nail tech delivered😄.</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cucmdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1cucefi</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Should I find a new nail tech???</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cucefi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1cuc9z7</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>What is a fair price for this?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kleecit9311d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1cuc97r</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Engagement manicure suggestions!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cuc97r/engagement_manicure_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1cubmfi</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Cake Nail I Made🎂</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cubmfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1cubjbb</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Best nail lamp specs?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cubjbb/best_nail_lamp_specs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1cuatoi</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>tried experimenting today</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuatoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1cuaml0</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Expressie "Express to Impress" </t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0og49a9r01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1cu9sjk</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Probably one of my fav sets ever 🤩</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8vcilt8l01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1cu9qxo</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Obsessed with this set ✨</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8n1911hxk01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1cu9q5d</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Pearl white with silver art ☁️</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu9q5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1cu9n0d</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>At-home acrylic overlay!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv48beb5k01d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1cu92p1</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Press ons for my birthday tomorrow</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu92p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1cu8inp</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Silver Lines</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3f00zn1c01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1cu8a3i</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Guess my favorite color?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqf55nvaa01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1cu89e8</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombre ✨ gel extension </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usf87vq5a01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1cu7l58</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>newest set on my natural nails :)</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu7l58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1cu6uq8</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>I love pink!</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu6uq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1cu6l33</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love how they looked </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddumf2q0yz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1cu6gyc</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Florals &amp; Chrome Farewell Spring Hello Summer</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu6gyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1cu51ut</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l68j19uqmz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1cu4vox</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>how much would you pay for this?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu4vox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1cu4uu7</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternatives to Dazzle Dry? </t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cu4uu7/alternatives_to_dazzle_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1cu4co8</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>I wanted octopus nails and my nail tech delivered 🐙</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c80hy0q2hz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1cu49j1</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Have nail biting problem… tips for growth? Embarrassing nail pic for context :(</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xmcn0vbgz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1cu443e</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Thought I'd try Chrome</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cu443e/thought_id_try_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1cu3vxl</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>I painted press on nail tips.</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lewz2cjwcz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1cu3t34</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Got my nails done ✨😍</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47k91yq6cz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1cu3po9</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Tipped my nail tech today😊</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpdovbjcbz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1cu3pd4</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Which shape for fake nails ?</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu3pd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1cu3l5x</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Fun nails</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu3l5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1cu3bqa</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>something about chocolate colored nails 🍫</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvsgjser7z0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1cu2plm</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>This lavender colour is so pretty ☺️</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn15n7q81z0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1cu2kih</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>French Pedi or All White Pedi with this Nail Set ?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5d1s9fpzy0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1cus044</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>How do I stop this? 😭</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/808wbh8j251d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1curze0</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Got my hands on my first bunch of Dany Vianna polishes and I thought they'd be perfect for a skittle manicure.</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3e55yf9251d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1curr5a</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Ghosts of Hecate &amp; Foxfire</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1curr5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1curiqr</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>ILNP collection</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1curiqr/ilnp_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1cuqs08</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Magnetics questions</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cuqs08/magnetics_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1cuo496</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Can the ILNP polish with glitter get gritty and get caught on clothes?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cuo496/can_the_ilnp_polish_with_glitter_get_gritty_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1cumgug</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Is it a topper or a full coverage glitter?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cumgug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1cuedca</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Just starting out</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aj5xkkvyi11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1cukzjt</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Stolen Ambrosia (mooncat) in direct sunlight</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blgywn8b031d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1cujxsy</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>This is what I wanted....</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cujxsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1cujrmc</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else have really unphotogenic nails? </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cujrmc/does_anyone_else_have_really_unphotogenic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1cujgut</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>One of my favorite holo glitters 🤩🧡</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/po3933t0n21d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1cujcky</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>When your nude polish is just too nude</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cujcky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1cuj0lo</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Blurring Base Coat</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cuj0lo/blurring_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1cui9z3</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Pic taken in the work bathroom stall 🧚🏻‍♀️🚽🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqpitkz2d21d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1cui1qq</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>sparkly rainbow french tip skittle ✨🌈</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cui1qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1cuhthw</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zoya sale </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cuhthw/zoya_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1cuh45e</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>My first magnetic!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuh45e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1cugym4</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>How often/long do you guys plan your manicures in advance?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cugym4/how_oftenlong_do_you_guys_plan_your_manicures_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1cughro</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>First stab at gradient nails</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ip64qvxwy11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1cufx0i</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tulips 🌷 </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9hxc6cfu11d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1cufv0y</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Mishipeshu by LynB Designs</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhamwtnzt11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1cufums</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Can't stop taking pictures of ILNP Flower Child!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cufums</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1cufccn</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Ghostly polishes are so mesmerizing</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s1kswho0q11d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1cufaoa</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Lumen Glass Teardrops</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfdr8k8pp11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1cuf851</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>I'm finally figuring out my undertones... behold my destash/reject pile! 🎨</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuf851</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1cuf5n7</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else bummed that Bluebird Lacquer switched their open date from today to 5/24 instead? </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cuf5n7/anyone_else_bummed_that_bluebird_lacquer_switched/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1cuf2uj</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>When the Sun Leaves</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njuj4880o11d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1cud3bz</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>What does a nice manicure symbolize to you?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cud3bz/what_does_a_nice_manicure_symbolize_to_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1cucnqn</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>This jelly is so gorgeous!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbyutj66611d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1cubrof</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>A combination I knew I needed 💎</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cubrof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1cubop3</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>OPI - Pearlcore</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhy37nzuy01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1cub75h</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>It’s such a crime that this polish was discontinued!!</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yulfrfbcv01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1cuak4g</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Silk Nail Wraps for the win!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t169wlirq01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1cua1ai</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>I think I found THE velvet mani technique</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e12r5m50n01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1cu9sev</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>My 11yo son got me nail polish for mother's day</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1qmit38l01d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1cu9dv6</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>La Vie En Rose</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu9dv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1cu90mz</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Holo jelly skittle</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu90mz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1cu8yn6</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Mercury in Retrograde - Velvet</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e0a6zgp8f01d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1cu80wb</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>This is my new favorite polish. Pictures don't do justice. Cirque - Mermaid Grotto</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu80wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1cu7m1p</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>What a Peach - KBShimmer</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu7m1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1cu77u7</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Makes any light crème a thermal.</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu77u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1cu7757</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Endlessly thickening top coat struggles</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cu7757/endlessly_thickening_top_coat_struggles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1cu5nrn</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your non-negotiable manicure steps? </t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cu5nrn/what_are_your_nonnegotiable_manicure_steps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1cu4o94</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>The Moolissa 🐄🖤🩷🤍</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu4o94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1cu4k6p</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Just a shoutout for Mooncat</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cu4k6p/just_a_shoutout_for_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1cu49v3</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Dupe request</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cu49v3/dupe_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1cu2xsv</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Mooncat ‘Flight of the Monarchs’ kinda disappointed me, so I made my own concoction</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cu2xsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1cu0c1y</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Moondust</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cu0c1y/moondust/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1cul79f</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cul79f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1cuifih</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>The first two photos were taken 3 years ago and these last two are very recent. I just wanna show you guys that practice=progress. Don't stop and keep up your hard work!!!</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuifih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1cuhshc</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Purple/Green foil with Gold Design</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuhshc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1cugfc6</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Marbled frenchies</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cugfc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1cufzsm</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Cat eye🔮✨</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cufzsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1cud90j</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Matching mani 😊</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cud90j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1cuchzr</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Loved the result</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aytvweaq411d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1cuce1d</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Nails for my puppy’s funeral, nails of sadness</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u4jah14411d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1cubuax</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Harry Potter nails</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cubuax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1cubndk</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>I Made A Cake Nail🎂🎂</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cubndk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1cu6r7n</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Nails in Korea</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gqcefzizz0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1cu09pw</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Pink and butterflies</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qvzoen47y0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1cu0332</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>looks not bad XD</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixev8lri4y0d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May 19 08:07:39 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_19.xlsx
+++ b/data/2024_05_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1135"/>
+  <dimension ref="A1:C1302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19728,6 +19728,2845 @@
         </is>
       </c>
     </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1cviqk9</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>The polishes i wore in April!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4frxn4045c1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1cvhteu</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Almost 4 hours of work, but it was worth it, I LOVE THEM.</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cowknm7ub1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1cvh600</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Found Some1 To Fix My Nails, Now They're Breaking Again--Why?</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cvh600/found_some1_to_fix_my_nails_now_theyre_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1cvgdav</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Did this gelx set on myself today</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqapcpnmdb1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1cvfsn2</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Dark set?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/621cer6h7b1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1cvfjms</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My First Set of Acrylics </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p54ghngv4b1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1cvfcop</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Fresh mani 💅✨</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv54nfcy2b1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1cvf5a1</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Did it myself ✨</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvf5a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1cvf2g2</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails, new color </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmkshatyza1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1cvez7b</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>They're stick ons but damn. Just wanted to share! 🤍</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rm6ad7u2za1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1cvep8q</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Groovy Fresh Set 🧡</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvep8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1cveiwh</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Super simple for a wedding 😁</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qcygehjua1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1cve396</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anytime I see my natural nails I want to commit to not putting dip on but then I do lolol! </t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ckwigxbqa1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1cve2jg</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>May nails</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cve2jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1cvdzjx</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>new set!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h085w7fcpa1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1cvdyum</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>What y’all think first time doing polygel 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jyxqyd5pa1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1cvdtgr</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I really like purple.</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r12zm2znna1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1cvdgnz</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>overly recommendations?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvdgnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1cvcscv</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Does this shade fit my tone?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvcscv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1cvcmro</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>I’m so happy with this dip set.</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvcmro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1cvcmop</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>new set 🤭</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvcmop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1cvchfk</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Something about classic French</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjuxkea5ba1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1cvc200</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>obsessed with my grad nails</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgvt1vz77a1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1cvbqsw</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Longest I've had, but I think I like it! </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7b9fvbf4a1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1cvbevv</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail glue bubbles </t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cvbevv/nail_glue_bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1cvbent</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Long term nail affair?!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f3372dd1a1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1cvbdwq</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Marble nails</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvbdwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1cvb9x4</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Are there specific brands of acrylic nails that are stronger than others?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cvb9x4/are_there_specific_brands_of_acrylic_nails_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1cvb6hm</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Feeling so fruity lately</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6603d1edz91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1cvb11v</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Bridgerton put me in the mood for florals 💙🩵🤍</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eusi1id2y91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1cvajvj</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Do these look bad?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvajvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1cvai75</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Missed my long nails</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvai75</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1cvaftp</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍒 </t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtjfxh6vs91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1cv9xek</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>The gurls are ready for summer ☀️</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9xek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1cv9ooz</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Still getting used to applying these gel stickers. But loving fun summer vibe.</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y4oit09m91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1cv9m8s</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Got my nails done yesterday!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4xsd27nl91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1cv9lbp</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Strawberry Nails 🍓</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9lbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1cv9i2i</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Aurora Chrome nails</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tzx9tdlkk91d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1cv9icf</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>{PR} LBH Sassy Sauce On a cold dark night</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9icf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1cv9hgd</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>abstractieeesssss!! 💜🍭</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqqjzxzhk91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1cv9g1d</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Nails with the girls</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9g1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1cv8qv2</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>New babies😍</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv8qv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1cv8qe5</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Tucan</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd5gfnm5e91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1cv8p9k</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Duck</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv8p9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1cv8kbz</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Plain and simple 🩷</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3muf88vrc91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1cv8a4v</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For my birthday </t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzmjcwwga91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1cv85u1</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>A disaster! What color do I change to?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edj2782i991d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1cv83rc</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>natural length! I love this color!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zahrcn71991d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1cv839f</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>my nail tech never disappoints 😤</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv839f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1cv7u13</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Easy way to accelerate soak off!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nppys6t691d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1cv7rc1</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>It’s Showtime! (DIY extensions)</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv7rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1cv7p5g</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Always loved this combo so I got it again!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/alzuve3j591d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1cv7bxi</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>My new set of press ons for the next couple of weeks 🙂‍↔️🩷</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv7bxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1cv7bim</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>First time getting gel x!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1gnny9k291d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1cv7alc</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>I started doing my own gel nails about 5 months ago. How am I doing?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv7alc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1cv7a6c</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Who has tried mooncat? Is the quality worth it. I’m in love with their cool colors but I’m always into gel more. </t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cv7a6c/who_has_tried_mooncat_is_the_quality_worth_it_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1cv7907</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>It’s definitely the press-ons. They make everyone’s hands look weird.</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ptfqboy191d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1cv6vlm</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>First time with chrome!</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh6ijwwwy81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1cv6uiw</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>I didn’t ask for the black tip and it was too late 🥲. Does it look ok? It really bugs me.</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv6uiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1cv6u9c</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>rate my nails!!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv6u9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1cv6t69</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>natural press on frenchies</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cv6t69/natural_press_on_frenchies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1cv6lqo</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Floral nails 💕</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv6lqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1cv660w</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Just left the salon with a fresh set and I couldn’t be happier</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv660w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1cv5fyz</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Why do people get Gel X professionally done when at-home application is so easy?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cv5fyz/why_do_people_get_gel_x_professionally_done_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1cv5bjk</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>My fresh red nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krtftfyem81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1cv54eu</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>It was just a hobby, but now I’m planning on becoming a nail tech/artist in the future.</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8bitjyvk81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1cv51ox</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>tried press on nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv51ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1cv4wry</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie Nails </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv4wry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1cv4tdz</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Is there any way to remove nail glue from fake nails without ruining them?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cv4tdz/is_there_any_way_to_remove_nail_glue_from_fake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1cv4diw</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Painted my nails for the first time in 3 years</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv4diw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1cv4crk</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>I’m in love with this design 💗</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6skbr7pe81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1cv46zq</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Just a better angle of all my nails for your viewing pleasure pt2</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv46zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1cv3y6y</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Natural nails with a gel manicure for only $38! I love her!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmyftwfhb81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1cv3xeo</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Marble🔥🫶🏽 </t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofbwzegbb81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1cv3rxi</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>All of these nail polishes were at my local Salvation Army store. They were $1.99 each at Walmart they are $10.99 I'm saving more than $100 with this hall. Brands are sally Hansen,salon perfect, and o.p.i</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbihr524a81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1cv3kwx</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Acrylic set with stamp &amp; hand-painted design</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu5evt3k881d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1cv3dz1</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Any tricks for doing your non dominant hand 😅</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/317iep01781d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1cv3atk</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just left the salon - Am I the only one thinking this is a bad mani? </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv3atk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1cv3a3q</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>First time using Builder Gel at home</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jbj3hh7681d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1cv2t78</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy with my progress. </t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5r71z84i281d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1cv2sfz</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>How to book</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv2sfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1cv2rxs</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Round 2💗🌌</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv2rxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1cv2kb0</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Princess pink gel manicure done at home 💖</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ivm6mbi081d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1cv24x4</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Looking for nail tech recs in the Boston area</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cv24x4/looking_for_nail_tech_recs_in_the_boston_area/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1cv241j</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Keep the vacation vibes going.. </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zqn4upww71d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1cv22oj</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>I’m French tip obsessed 💅</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv22oj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1cv215a</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Another cute set</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv215a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1cv1wpy</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Tried to do a cool thing</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv1wpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1cv1pfk</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Did my nails baby pink and hated it so I slapped on some aurora powder. I think I’m addicted</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv1pfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1cv1n1w</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>I feel like these would be pretty as bridal nails. Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv1n1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1cv0r1c</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>best quality press ons?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cv0r1c/best_quality_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1cv0oq9</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made it!! </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cv0oq9/i_made_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1cv07jj</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Nail recommendations (Color and shape)</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y7c76bgh71d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1cv04cm</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and pink </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/DdMdQqF.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1cuzzq0</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Summer nails finally on!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuzzq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1cuzc4g</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Tell me you do your own nails without telling me you do your own nails….</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1gyqom7a71d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1cuzaec</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Can’t decide if I like this design/color combo or not</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuzaec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1cuyu1m</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>black french tips are so elegant looking 😊🖤</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5o2sbk0671d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1cuytsg</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Idk how to feel about press ons. I think they make my hands look a little weird.</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va1qjkxx571d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1cuysv9</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Nails for prom</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cuysv9/nails_for_prom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1cvi0yu</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Bought this from a home salon in Asia because I loved the color so much, any idea?</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvi0yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1cvhyma</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Sally Hansen x LoveShackFancy</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cvhyma/sally_hansen_x_loveshackfancy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1cvhtuu</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Almost 4 hours of work, but it was worth it, I LOVE THEM.</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wje14x3cub1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1cvgimj</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>ILNP High Voltage 💙💜</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvgimj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1cvefob</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>My new favorite purple polish. And that's saying something!</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvefob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1cvdwy0</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bowling casualty </t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzrbmqwloa1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1cvduyo</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Was in need of a palate cleanser</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkmi2p63oa1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1cvdst8</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Can I attach acrylic nails and apply regular polish without buffing down the actual nails?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cvdst8/can_i_attach_acrylic_nails_and_apply_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1cvd6f3</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Felt cute</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpuyz56kha1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1cvd2ll</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>It took me three different tries to get the layering combo I wanted 🫠</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krsi2v6lga1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1cvczar</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Essie's Bikini So Teeny</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sxc4xaqfa1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1cvcvu4</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Tried my hand (pun lol) at some accent nails :)</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvcvu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1cvck6m</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Fell onto the Bluebell wagon~~~</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23vgydmuba1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1cvchgd</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Iris You Were Here</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvchgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1cvc3v4</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Polish Swatch Dot problems</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cvc3v4/polish_swatch_dot_problems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1cvc05f</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Transforming in different lighting and angles! 🌸</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvc05f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1cvalc5</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Does this expire?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8nq1lq9u91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1cun04b</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Just a question</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cun04b/just_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1curno3</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Deformed thumb nail</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1curno3/deformed_thumb_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1cva3aa</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>House of Hades comparisons</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cva3aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1cv9whc</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Sally Hansen x Ring Pop</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9whc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1cv9mul</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>{PR} LBH | Sassy Sauce | On a dark cold night</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9mul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1cv92az</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Zoisite by LynBDesigns</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv92az</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1cv8cym</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>LynBDesigns “Gentleman Pirate”</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv8cym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1cv83ch</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>It’s here!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv83ch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1cv7plo</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Juicy jellies</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv7plo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1cv7nhm</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Does anyone else like to do more silly/whimsical nail art?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnsdfkxb591d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1cv7c7v</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Flower child</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv7c7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1cv6zo5</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Chanel Rouge Noir/Essie Wicked but warmer?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cv6zo5/chanel_rouge_noiressie_wicked_but_warmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1cv6vma</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Probably my favorite from my Cirque lucky bag</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny2as1xwy81d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1cv6kka</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Indomitable</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv6kka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1cv66lx</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>I need more shades with a soft gold shimmer 🤩</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv66lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1cv5igx</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Orly Hot Pursuit 🪸</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/luxeyhixn81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1cv52bf</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sale alert 🚨 50% off at Dreamland Lacquer </t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ookx3wnek81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1cv45l3</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>A Mooncat mani to tide me over until my order arrives :)</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id01uih3d81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1cv3fm8</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>A new-to-me shade from Mooncat just arrived! Mooncat - Maelstrom</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vgc9m4e781d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1cv2rgy</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>First time DIY dip</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zevqdk33281d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1cv1kgg</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>First time trying nail art</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv1kgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1cv1juz</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Retro pastel flowers</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi1tbvjhs71d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1cv1gyu</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>I have some polishes that dry matte or textured (on purpose). If you're supposed to use a top coat, what's the purpose of having these special finishes?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cv1gyu/i_have_some_polishes_that_dry_matte_or_textured/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1cv1b0p</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>First attempt at this style</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv1b0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1cv16bi</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>I think I found my perfect nude!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0pl6aibp71d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1cuzlt6</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>You already know what it is 🌸</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuzlt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1cuzjx1</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Death Valley Nails- Suddenly🔥</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuzjx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1cuz1n0</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Holo taco rainbow bundle</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cuz1n0/holo_taco_rainbow_bundle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1cuyoq1</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>The shifts 🤩</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuyoq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1cuya7n</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Help me find dupes of these Lights Lacquer shades</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w642shqz071d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1cuxu5i</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Glitter grabber?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cuxu5i/glitter_grabber/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1cuwukk</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Does anyone know what this shade is? I tried finding it thru the link on Pinterest, but got the 404 error code 😔</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3q91m13o61d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1cuv47i</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thought that I'd try Chrome </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuv47i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1cuur4i</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>And another one 😭</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6c2i8d3261d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1cvirlu</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Help please!</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvirlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1cvikvj</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Design I’m Doing For Someone </t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asbd8ku63c1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1cvh9i7</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Basic need for a nail artist.... My Girlfriend is so Obsessed with her nailart channel she buys all of these 💀💀😅</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leeqn4gvnb1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1cvfalx</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cvfalx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1cvd61t</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Retro vibes ✌🏻✨</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvy2721hha1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1cvcv8p</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>My new fav custom !!</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyijnfrnea1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1cvbjtf</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>3D sculpted dart frog the hubby!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lzvjt7o2a1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1cvayn0</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Minnie n Micky🖤🤍</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnpigasix91d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1cv9yq2</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>The gurls are ready for summer ☀️</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9yq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1cv9qus</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Strawberry Nails 🍓</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv9qus</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1cv7k0x</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>It’s showtime!</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cv7k0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1cv7826</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmbavinq191d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1cv4amg</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>metal designs are my favorite 🤩</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26dvrfr7e81d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1cv2oiv</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy with my French tips! </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3gqox6g181d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1cuyrnz</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>full set</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuyrnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1cuwbje</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Antique Angelical set</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cuwbje</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>